<commit_message>
data classes and datetime shit
</commit_message>
<xml_diff>
--- a/test2.xlsx
+++ b/test2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henryvecchione/Desktop/Home/myboathouse2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B693D17C-39C0-E041-A940-0AE7CD99B6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C8B2DC-5E6D-7048-8274-B6713D6B3636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -88,6 +88,15 @@
     <t>gorvy</t>
   </si>
   <si>
+    <t>r 24</t>
+  </si>
+  <si>
+    <t>r30</t>
+  </si>
+  <si>
+    <t>r32</t>
+  </si>
+  <si>
     <t>6000m</t>
   </si>
   <si>
@@ -95,15 +104,6 @@
   </si>
   <si>
     <t>2000m</t>
-  </si>
-  <si>
-    <t>r 24</t>
-  </si>
-  <si>
-    <t>r30</t>
-  </si>
-  <si>
-    <t>r32</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -508,13 +508,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -525,13 +525,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>